<commit_message>
Revert "CommonDataStructure extended to work with WF task. Bug fixed when retrieving forces from NSx."
This reverts commit 7c8e22d2107894e003ba1de0ef185d6269124511, reversing
changes made to 6298c6643bce0d16c44601a5e1db97edf9a64288.
</commit_message>
<xml_diff>
--- a/@commonDataStructure/trialTableLabels.xlsx
+++ b/@commonDataStructure/trialTableLabels.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="85">
   <si>
     <t>label</t>
   </si>
@@ -59,199 +59,190 @@
     <t>xOffset</t>
   </si>
   <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>yOffset</t>
+  </si>
+  <si>
+    <t>timing</t>
+  </si>
+  <si>
+    <t>ctrTgtOnTime</t>
+  </si>
+  <si>
+    <t>time from the start of the file when the center target turns on after the start of the trial</t>
+  </si>
+  <si>
+    <t>ctrHold</t>
+  </si>
+  <si>
+    <t>time the monkey had to hold in the center before the outer target appeared</t>
+  </si>
+  <si>
+    <t>tgtOnTime</t>
+  </si>
+  <si>
+    <t>time from the start of the file that the target appeared. For trials with multiple target onsets this may have multiple sub columns</t>
+  </si>
+  <si>
+    <t>delayHold</t>
+  </si>
+  <si>
+    <t>time in seconds the monkey had to wait after target appearance before go cue</t>
+  </si>
+  <si>
+    <t>goCueTime</t>
+  </si>
+  <si>
+    <t>time from the start of the file of the go cue</t>
+  </si>
+  <si>
+    <t>movePeriod</t>
+  </si>
+  <si>
+    <t>the time window for movement. Does not use moveTime otherwise the value would be timeshifted when merging trial tables</t>
+  </si>
+  <si>
+    <t>bumps</t>
+  </si>
+  <si>
+    <t>bumpTime</t>
+  </si>
+  <si>
+    <t>time from the start of the file of the bump</t>
+  </si>
+  <si>
+    <t>bumpLatency</t>
+  </si>
+  <si>
+    <t>time from the start of the phase that the bump occurred, for trials with multiple bumps this table column may contain multiple sub-columns</t>
+  </si>
+  <si>
+    <t>ctrHoldBump</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>was there a bump in the center hold</t>
+  </si>
+  <si>
+    <t>delayBump</t>
+  </si>
+  <si>
+    <t>was there a bump in the delay</t>
+  </si>
+  <si>
+    <t>moveBump</t>
+  </si>
+  <si>
+    <t>was there a bump in the move</t>
+  </si>
+  <si>
+    <t>bumpID</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>0-15 value that is the bump code sent by XPC</t>
+  </si>
+  <si>
+    <t>bumpDir</t>
+  </si>
+  <si>
+    <t>deg</t>
+  </si>
+  <si>
+    <t>bump angle in degrees</t>
+  </si>
+  <si>
+    <t>bumpRisePeriod</t>
+  </si>
+  <si>
+    <t>time the bump takes to go from 0N to peak force</t>
+  </si>
+  <si>
+    <t>bumpHoldPeriod</t>
+  </si>
+  <si>
+    <t>time the bump holds at peak force</t>
+  </si>
+  <si>
+    <t>bumpMagnitude</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>peak force of the bump</t>
+  </si>
+  <si>
+    <t>targets</t>
+  </si>
+  <si>
+    <t>numTgt</t>
+  </si>
+  <si>
+    <t>number of targets shown during a given trial. THIS IS NOT THE NUMBER OF DIFFERENT TARGETS IN THE SESSION</t>
+  </si>
+  <si>
+    <t>tgtID</t>
+  </si>
+  <si>
+    <t>0-15 value that is the code of the target on word sent by XPC</t>
+  </si>
+  <si>
+    <t>tgtCorners</t>
+  </si>
+  <si>
+    <t>1x4*numTgt float</t>
+  </si>
+  <si>
+    <t>x-y pairs for the upper right and lower left corners of the targets. For tasks with more than one target, this entry has 4xnumTgts elements</t>
+  </si>
+  <si>
+    <t>tgtDir</t>
+  </si>
+  <si>
+    <t>direction of target in degrees. Right is 0</t>
+  </si>
+  <si>
+    <t>tgtCtr</t>
+  </si>
+  <si>
+    <t>1x2*numTgt float</t>
+  </si>
+  <si>
+    <t>x-y pairs for the center of each target. This table column has 2*numTgt sub columns</t>
+  </si>
+  <si>
+    <t>numTgtAttempted</t>
+  </si>
+  <si>
+    <t>number of targets the monkey tried during the trial</t>
+  </si>
+  <si>
+    <t>tgtSize</t>
+  </si>
+  <si>
+    <t>for circleTargets, the diameter of the target. For squareTargets the width of the square</t>
+  </si>
+  <si>
+    <t>cursor</t>
+  </si>
+  <si>
+    <t>hideCursor</t>
+  </si>
+  <si>
+    <t>flag indicating whether the cursor was hidden on this trial</t>
+  </si>
+  <si>
+    <t>hideCursorMin</t>
+  </si>
+  <si>
     <t>cm</t>
-  </si>
-  <si>
-    <t>offset of cursor from robot axis in cm. Motor spindles are (0,0)</t>
-  </si>
-  <si>
-    <t>yOffset</t>
-  </si>
-  <si>
-    <t>timing</t>
-  </si>
-  <si>
-    <t>ctrTgtOnTime</t>
-  </si>
-  <si>
-    <t>time from the start of the file when the center target turns on after the start of the trial</t>
-  </si>
-  <si>
-    <t>ctrHold</t>
-  </si>
-  <si>
-    <t>time the monkey had to hold in the center before the outer target appeared</t>
-  </si>
-  <si>
-    <t>tgtOnTime</t>
-  </si>
-  <si>
-    <t>time from the start of the file that the target appeared. For trials with multiple target onsets this may have multiple sub columns</t>
-  </si>
-  <si>
-    <t>delayHold</t>
-  </si>
-  <si>
-    <t>time in seconds the monkey had to wait after target appearance before go cue</t>
-  </si>
-  <si>
-    <t>tgtHoldTime</t>
-  </si>
-  <si>
-    <t>time in seconds the monkey had to hold in the outer target before reward.</t>
-  </si>
-  <si>
-    <t>goCueTime</t>
-  </si>
-  <si>
-    <t>time from the start of the file of the go cue. In the case of RW or other tasks with multiple cues in a trial, this table column will have multiple sub-columns, one for each cue</t>
-  </si>
-  <si>
-    <t>movePeriod</t>
-  </si>
-  <si>
-    <t>the time window for movement. Does not use moveTime otherwise the value would be timeshifted when merging trial tables</t>
-  </si>
-  <si>
-    <t>bumps</t>
-  </si>
-  <si>
-    <t>bumpTime</t>
-  </si>
-  <si>
-    <t>time from the start of the file of the bump</t>
-  </si>
-  <si>
-    <t>bumpLatency</t>
-  </si>
-  <si>
-    <t>time from the start of the phase that the bump occurred, for trials with multiple bumps this table column may contain multiple sub-columns</t>
-  </si>
-  <si>
-    <t>ctrHoldBump</t>
-  </si>
-  <si>
-    <t>bool</t>
-  </si>
-  <si>
-    <t>was there a bump in the center hold</t>
-  </si>
-  <si>
-    <t>delayBump</t>
-  </si>
-  <si>
-    <t>was there a bump in the delay</t>
-  </si>
-  <si>
-    <t>moveBump</t>
-  </si>
-  <si>
-    <t>was there a bump in the move</t>
-  </si>
-  <si>
-    <t>bumpID</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>0-15 value that is the bump code sent by XPC</t>
-  </si>
-  <si>
-    <t>bumpDir</t>
-  </si>
-  <si>
-    <t>deg</t>
-  </si>
-  <si>
-    <t>bump angle in degrees</t>
-  </si>
-  <si>
-    <t>bumpRisePeriod</t>
-  </si>
-  <si>
-    <t>time the bump takes to go from 0N to peak force</t>
-  </si>
-  <si>
-    <t>bumpHoldPeriod</t>
-  </si>
-  <si>
-    <t>time the bump holds at peak force</t>
-  </si>
-  <si>
-    <t>bumpMagnitude</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>peak force of the bump</t>
-  </si>
-  <si>
-    <t>targets</t>
-  </si>
-  <si>
-    <t>numTgt</t>
-  </si>
-  <si>
-    <t>number of targets shown during a given trial. THIS IS NOT THE NUMBER OF DIFFERENT TARGETS IN THE SESSION</t>
-  </si>
-  <si>
-    <t>tgtID</t>
-  </si>
-  <si>
-    <t>0-15 value that is the code of the target on word sent by XPC</t>
-  </si>
-  <si>
-    <t>tgtCorners</t>
-  </si>
-  <si>
-    <t>1x4*numTgt float</t>
-  </si>
-  <si>
-    <t>x-y pairs for the upper right and lower left corners of the targets. For tasks with more than one target, this entry has 4xnumTgts elements</t>
-  </si>
-  <si>
-    <t>tgtDir</t>
-  </si>
-  <si>
-    <t>float</t>
-  </si>
-  <si>
-    <t>direction of target in degrees. Right is 0</t>
-  </si>
-  <si>
-    <t>tgtCtr</t>
-  </si>
-  <si>
-    <t>1x2*numTgt float</t>
-  </si>
-  <si>
-    <t>x-y pairs for the center of each target. This table column has 2*numTgt sub columns</t>
-  </si>
-  <si>
-    <t>numTgtAttempted</t>
-  </si>
-  <si>
-    <t>number of targets the monkey tried during the trial</t>
-  </si>
-  <si>
-    <t>tgtSize</t>
-  </si>
-  <si>
-    <t>for circleTargets, the diameter of the target. For squareTargets the width of the square</t>
-  </si>
-  <si>
-    <t>cursor</t>
-  </si>
-  <si>
-    <t>hideCursor</t>
-  </si>
-  <si>
-    <t>flag indicating whether the cursor was hidden on this trial</t>
-  </si>
-  <si>
-    <t>hideCursorMin</t>
   </si>
   <si>
     <t>minimum radius from the center of the workspace before the cursor will be hidden</t>
@@ -451,7 +442,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -526,6 +517,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -609,17 +604,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2834008097166"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5748987854251"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="146.63967611336"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="129.141700404858"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.53441295546559"/>
   </cols>
   <sheetData>
@@ -681,27 +676,23 @@
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>15</v>
-      </c>
+      <c r="C7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>15</v>
-      </c>
+      <c r="C8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6"/>
@@ -715,118 +706,118 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>18</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>20</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>22</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="15" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="13" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="s">
+      <c r="B17" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="15" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="16" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
+      <c r="B18" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="15" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="s">
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="18" t="s">
+      <c r="B22" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="15" t="s">
         <v>33</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>5</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>36</v>
@@ -837,29 +828,29 @@
         <v>37</v>
       </c>
       <c r="B25" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>38</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="15" t="s">
         <v>40</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="14" t="s">
         <v>42</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>38</v>
       </c>
       <c r="C27" s="15" t="s">
         <v>43</v>
@@ -881,69 +872,69 @@
         <v>47</v>
       </c>
       <c r="B29" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="15" t="s">
         <v>48</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="15" t="s">
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="16" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="13" t="s">
+      <c r="B31" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="16" t="s">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="B34" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="15" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="15" t="s">
         <v>58</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="14" t="s">
         <v>60</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>45</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>61</v>
@@ -954,97 +945,97 @@
         <v>62</v>
       </c>
       <c r="B37" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="15" t="s">
         <v>63</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="C38" s="15" t="s">
         <v>66</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="14" t="s">
+    </row>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="B40" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="18" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="13" t="s">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B40" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C40" s="15" t="s">
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="16" t="s">
+      <c r="B43" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="B43" s="19"/>
-      <c r="C43" s="19"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B45" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" s="0" t="s">
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C47" s="0" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="B46" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C46" s="0" t="s">
+      <c r="B48" s="0" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="s">
         <v>82</v>
       </c>
@@ -1054,21 +1045,10 @@
         <v>83</v>
       </c>
       <c r="B49" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1076,9 +1056,9 @@
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A42:C42"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Revert (for real this time) back to a good commit
</commit_message>
<xml_diff>
--- a/@commonDataStructure/trialTableLabels.xlsx
+++ b/@commonDataStructure/trialTableLabels.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="88">
   <si>
     <t>label</t>
   </si>
@@ -59,153 +59,165 @@
     <t>xOffset</t>
   </si>
   <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>offset of cursor from robot axis in cm. Motor spindles are (0,0)</t>
+  </si>
+  <si>
+    <t>yOffset</t>
+  </si>
+  <si>
+    <t>timing</t>
+  </si>
+  <si>
+    <t>ctrTgtOnTime</t>
+  </si>
+  <si>
+    <t>time from the start of the file when the center target turns on after the start of the trial</t>
+  </si>
+  <si>
+    <t>ctrHold</t>
+  </si>
+  <si>
+    <t>time the monkey had to hold in the center before the outer target appeared</t>
+  </si>
+  <si>
+    <t>tgtOnTime</t>
+  </si>
+  <si>
+    <t>time from the start of the file that the target appeared. For trials with multiple target onsets this may have multiple sub columns</t>
+  </si>
+  <si>
+    <t>delayHold</t>
+  </si>
+  <si>
+    <t>time in seconds the monkey had to wait after target appearance before go cue</t>
+  </si>
+  <si>
+    <t>tgtHoldTime</t>
+  </si>
+  <si>
+    <t>time in seconds the monkey had to hold in the outer target before reward.</t>
+  </si>
+  <si>
+    <t>goCueTime</t>
+  </si>
+  <si>
+    <t>time from the start of the file of the go cue. In the case of RW or other tasks with multiple cues in a trial, this table column will have multiple sub-columns, one for each cue</t>
+  </si>
+  <si>
+    <t>movePeriod</t>
+  </si>
+  <si>
+    <t>the time window for movement. Does not use moveTime otherwise the value would be timeshifted when merging trial tables</t>
+  </si>
+  <si>
+    <t>bumps</t>
+  </si>
+  <si>
+    <t>bumpTime</t>
+  </si>
+  <si>
+    <t>time from the start of the file of the bump</t>
+  </si>
+  <si>
+    <t>bumpLatency</t>
+  </si>
+  <si>
+    <t>time from the start of the phase that the bump occurred, for trials with multiple bumps this table column may contain multiple sub-columns</t>
+  </si>
+  <si>
+    <t>ctrHoldBump</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>was there a bump in the center hold</t>
+  </si>
+  <si>
+    <t>delayBump</t>
+  </si>
+  <si>
+    <t>was there a bump in the delay</t>
+  </si>
+  <si>
+    <t>moveBump</t>
+  </si>
+  <si>
+    <t>was there a bump in the move</t>
+  </si>
+  <si>
+    <t>bumpID</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>0-15 value that is the bump code sent by XPC</t>
+  </si>
+  <si>
+    <t>bumpDir</t>
+  </si>
+  <si>
+    <t>deg</t>
+  </si>
+  <si>
+    <t>bump angle in degrees</t>
+  </si>
+  <si>
+    <t>bumpRisePeriod</t>
+  </si>
+  <si>
+    <t>time the bump takes to go from 0N to peak force</t>
+  </si>
+  <si>
+    <t>bumpHoldPeriod</t>
+  </si>
+  <si>
+    <t>time the bump holds at peak force</t>
+  </si>
+  <si>
+    <t>bumpMagnitude</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>peak force of the bump</t>
+  </si>
+  <si>
+    <t>targets</t>
+  </si>
+  <si>
+    <t>numTgt</t>
+  </si>
+  <si>
+    <t>number of targets shown during a given trial. THIS IS NOT THE NUMBER OF DIFFERENT TARGETS IN THE SESSION</t>
+  </si>
+  <si>
+    <t>tgtID</t>
+  </si>
+  <si>
+    <t>0-15 value that is the code of the target on word sent by XPC</t>
+  </si>
+  <si>
+    <t>tgtCorners</t>
+  </si>
+  <si>
+    <t>1x4*numTgt float</t>
+  </si>
+  <si>
+    <t>x-y pairs for the upper right and lower left corners of the targets. For tasks with more than one target, this entry has 4xnumTgts elements</t>
+  </si>
+  <si>
+    <t>tgtDir</t>
+  </si>
+  <si>
     <t>float</t>
   </si>
   <si>
-    <t>yOffset</t>
-  </si>
-  <si>
-    <t>timing</t>
-  </si>
-  <si>
-    <t>ctrTgtOnTime</t>
-  </si>
-  <si>
-    <t>time from the start of the file when the center target turns on after the start of the trial</t>
-  </si>
-  <si>
-    <t>ctrHold</t>
-  </si>
-  <si>
-    <t>time the monkey had to hold in the center before the outer target appeared</t>
-  </si>
-  <si>
-    <t>tgtOnTime</t>
-  </si>
-  <si>
-    <t>time from the start of the file that the target appeared. For trials with multiple target onsets this may have multiple sub columns</t>
-  </si>
-  <si>
-    <t>delayHold</t>
-  </si>
-  <si>
-    <t>time in seconds the monkey had to wait after target appearance before go cue</t>
-  </si>
-  <si>
-    <t>goCueTime</t>
-  </si>
-  <si>
-    <t>time from the start of the file of the go cue</t>
-  </si>
-  <si>
-    <t>movePeriod</t>
-  </si>
-  <si>
-    <t>the time window for movement. Does not use moveTime otherwise the value would be timeshifted when merging trial tables</t>
-  </si>
-  <si>
-    <t>bumps</t>
-  </si>
-  <si>
-    <t>bumpTime</t>
-  </si>
-  <si>
-    <t>time from the start of the file of the bump</t>
-  </si>
-  <si>
-    <t>bumpLatency</t>
-  </si>
-  <si>
-    <t>time from the start of the phase that the bump occurred, for trials with multiple bumps this table column may contain multiple sub-columns</t>
-  </si>
-  <si>
-    <t>ctrHoldBump</t>
-  </si>
-  <si>
-    <t>bool</t>
-  </si>
-  <si>
-    <t>was there a bump in the center hold</t>
-  </si>
-  <si>
-    <t>delayBump</t>
-  </si>
-  <si>
-    <t>was there a bump in the delay</t>
-  </si>
-  <si>
-    <t>moveBump</t>
-  </si>
-  <si>
-    <t>was there a bump in the move</t>
-  </si>
-  <si>
-    <t>bumpID</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>0-15 value that is the bump code sent by XPC</t>
-  </si>
-  <si>
-    <t>bumpDir</t>
-  </si>
-  <si>
-    <t>deg</t>
-  </si>
-  <si>
-    <t>bump angle in degrees</t>
-  </si>
-  <si>
-    <t>bumpRisePeriod</t>
-  </si>
-  <si>
-    <t>time the bump takes to go from 0N to peak force</t>
-  </si>
-  <si>
-    <t>bumpHoldPeriod</t>
-  </si>
-  <si>
-    <t>time the bump holds at peak force</t>
-  </si>
-  <si>
-    <t>bumpMagnitude</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>peak force of the bump</t>
-  </si>
-  <si>
-    <t>targets</t>
-  </si>
-  <si>
-    <t>numTgt</t>
-  </si>
-  <si>
-    <t>number of targets shown during a given trial. THIS IS NOT THE NUMBER OF DIFFERENT TARGETS IN THE SESSION</t>
-  </si>
-  <si>
-    <t>tgtID</t>
-  </si>
-  <si>
-    <t>0-15 value that is the code of the target on word sent by XPC</t>
-  </si>
-  <si>
-    <t>tgtCorners</t>
-  </si>
-  <si>
-    <t>1x4*numTgt float</t>
-  </si>
-  <si>
-    <t>x-y pairs for the upper right and lower left corners of the targets. For tasks with more than one target, this entry has 4xnumTgts elements</t>
-  </si>
-  <si>
-    <t>tgtDir</t>
-  </si>
-  <si>
     <t>direction of target in degrees. Right is 0</t>
   </si>
   <si>
@@ -240,9 +252,6 @@
   </si>
   <si>
     <t>hideCursorMin</t>
-  </si>
-  <si>
-    <t>cm</t>
   </si>
   <si>
     <t>minimum radius from the center of the workspace before the cursor will be hidden</t>
@@ -442,7 +451,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -517,10 +526,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -604,17 +609,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2834008097166"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5748987854251"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="129.141700404858"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="146.63967611336"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.53441295546559"/>
   </cols>
   <sheetData>
@@ -676,23 +681,27 @@
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6"/>
@@ -706,118 +715,118 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="18" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="13" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="19" t="s">
+      <c r="B18" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-    </row>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>31</v>
-      </c>
+      <c r="A22" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>36</v>
@@ -828,29 +837,29 @@
         <v>37</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C27" s="15" t="s">
         <v>43</v>
@@ -872,69 +881,69 @@
         <v>47</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B30" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="17" t="s">
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="B31" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="15" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="19" t="s">
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
+      <c r="B32" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>56</v>
-      </c>
+      <c r="A34" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>61</v>
@@ -945,97 +954,97 @@
         <v>62</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" s="18" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="20" t="s">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
+      <c r="B40" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>73</v>
-      </c>
+      <c r="A43" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="0" t="s">
         <v>79</v>
       </c>
     </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>81</v>
-      </c>
       <c r="C48" s="0" t="s">
         <v>82</v>
       </c>
@@ -1045,10 +1054,21 @@
         <v>83</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C49" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" s="0" t="s">
         <v>84</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1056,9 +1076,9 @@
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A43:C43"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>